<commit_message>
Removed the tokenize expressions. Updated testing and the testcases as well.
</commit_message>
<xml_diff>
--- a/TESTCASES_SIMPLIFICATION.xlsx
+++ b/TESTCASES_SIMPLIFICATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/a_n_lindelauf_student_tue_nl/Documents/Documents/TUe/Year 3/Q2/Mathematical modelling/Mathematical-Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{EE87A0B8-AD9A-4CE2-B609-79C8428943CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6281FD8A-EDE9-413D-85B9-FCE16BBBB0FB}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{EE87A0B8-AD9A-4CE2-B609-79C8428943CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FE22D1-AF9D-47A3-8422-256344143B51}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{75F50C61-28CB-4ED2-901F-FE78C52DBAD5}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>ab</t>
   </si>
   <si>
-    <t>2a</t>
-  </si>
-  <si>
     <t>2ab + ac</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>17 b^4 + 2 a + 4^(1 + 2 a) + 18</t>
+  </si>
+  <si>
+    <t>2x</t>
   </si>
 </sst>
 </file>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9F256-B036-4CF9-B217-A6DE0B7F2A35}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="143" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +743,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -791,7 +791,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,7 +807,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -839,7 +839,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -847,7 +847,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -863,7 +863,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -871,7 +871,7 @@
         <v>-5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -879,7 +879,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -895,7 +895,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Instead of doing a simplification 10 times, we keep simplifying the expression until it doesn't get more simple.
</commit_message>
<xml_diff>
--- a/TESTCASES_SIMPLIFICATION.xlsx
+++ b/TESTCASES_SIMPLIFICATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/a_n_lindelauf_student_tue_nl/Documents/Documents/TUe/Year 3/Q2/Mathematical modelling/Mathematical-Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{EE87A0B8-AD9A-4CE2-B609-79C8428943CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FE22D1-AF9D-47A3-8422-256344143B51}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{EE87A0B8-AD9A-4CE2-B609-79C8428943CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C458FDE0-8EE1-4BA8-8B35-70458886F7B9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{75F50C61-28CB-4ED2-901F-FE78C52DBAD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>2 + 1</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>2x</t>
+  </si>
+  <si>
+    <t>3 * x/y</t>
+  </si>
+  <si>
+    <t>x/y + (2x)/y</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9F256-B036-4CF9-B217-A6DE0B7F2A35}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="143" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,6 +920,14 @@
         <v>46</v>
       </c>
     </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed test case 5
</commit_message>
<xml_diff>
--- a/TESTCASES_SIMPLIFICATION.xlsx
+++ b/TESTCASES_SIMPLIFICATION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/a_n_lindelauf_student_tue_nl/Documents/Documents/TUe/Year 3/Q2/Mathematical modelling/Mathematical-Modelling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/n_v_d_poel_student_tue_nl/Documents/Desktop/Mathematical-Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{EE87A0B8-AD9A-4CE2-B609-79C8428943CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C2741B-FC1F-4632-9457-A5769EE60C98}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{EE87A0B8-AD9A-4CE2-B609-79C8428943CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1BB8279-B7EE-4E60-AA49-66316BDC60D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{75F50C61-28CB-4ED2-901F-FE78C52DBAD5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75F50C61-28CB-4ED2-901F-FE78C52DBAD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>( a * b * c ) ^ d</t>
   </si>
   <si>
-    <t>a ^ (b ^ (c ^ d))</t>
-  </si>
-  <si>
     <t>3(a+3)</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>4ab/(2^3*2*t+t)+ab4/(t+(8+8)t)</t>
+  </si>
+  <si>
+    <t>((a^b)^c)^d</t>
   </si>
 </sst>
 </file>
@@ -280,7 +280,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9F256-B036-4CF9-B217-A6DE0B7F2A35}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="143" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,10 +626,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -653,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -661,76 +661,76 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>46656</v>
@@ -738,138 +738,138 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -877,55 +877,55 @@
         <v>-5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>